<commit_message>
Added STFT and RESNET code for the Upper and Lower dataset
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project start2\Dataset\Lower Limb Data\Python processing  &amp; results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project start2\Dataset\Codes\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9034A8-575B-4303-B284-733ACD03B376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9CF99B-701D-4F65-B6AF-76FF59E5541F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{07C07F02-9507-4FBE-9AE4-8E7E1B112653}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{07C07F02-9507-4FBE-9AE4-8E7E1B112653}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="22">
   <si>
     <t>BackStep</t>
   </si>
@@ -101,6 +102,9 @@
   <si>
     <t>SVM</t>
   </si>
+  <si>
+    <t>Max/Min</t>
+  </si>
 </sst>
 </file>
 
@@ -147,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -156,10 +160,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,52 +490,52 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:20" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="L2" s="3" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="L2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1479,52 +1486,52 @@
       </c>
     </row>
     <row r="20" spans="1:20" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="L21" s="3" t="s">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="L21" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -2490,61 +2497,61 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA782662-3728-4105-B233-531D5B1EC0B1}">
-  <dimension ref="A1:AD35"/>
+  <dimension ref="A1:AD36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H12" workbookViewId="0">
-      <selection activeCell="Z36" sqref="Z36"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E42" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:20" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
       <c r="I2" s="2"/>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="5"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="4"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -2616,11 +2623,11 @@
         <v>0.82</v>
       </c>
       <c r="G4">
-        <f>ROUND(AVERAGE(B4:F4),2)</f>
+        <f t="shared" ref="G4:G15" si="0">ROUND(AVERAGE(B4:F4),2)</f>
         <v>0.8</v>
       </c>
       <c r="H4">
-        <f>ROUND(_xlfn.STDEV.S(B4,B4:F4),2)</f>
+        <f t="shared" ref="H4:H15" si="1">ROUND(_xlfn.STDEV.S(B4,B4:F4),2)</f>
         <v>0.02</v>
       </c>
       <c r="L4">
@@ -2642,11 +2649,11 @@
         <v>0.75</v>
       </c>
       <c r="R4">
-        <f>ROUND(AVERAGE(M4:Q4),2)</f>
+        <f t="shared" ref="R4:R15" si="2">ROUND(AVERAGE(M4:Q4),2)</f>
         <v>0.78</v>
       </c>
       <c r="S4">
-        <f>ROUND(_xlfn.STDEV.S(M4,M4:Q4),2)</f>
+        <f t="shared" ref="S4:S15" si="3">ROUND(_xlfn.STDEV.S(M4,M4:Q4),2)</f>
         <v>0.04</v>
       </c>
     </row>
@@ -2670,11 +2677,11 @@
         <v>0.76</v>
       </c>
       <c r="G5">
-        <f>ROUND(AVERAGE(B5:F5),2)</f>
+        <f t="shared" si="0"/>
         <v>0.81</v>
       </c>
       <c r="H5">
-        <f>ROUND(_xlfn.STDEV.S(B5,B5:F5),2)</f>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="L5">
@@ -2696,11 +2703,11 @@
         <v>0.74</v>
       </c>
       <c r="R5">
-        <f>ROUND(AVERAGE(M5:Q5),2)</f>
+        <f t="shared" si="2"/>
         <v>0.77</v>
       </c>
       <c r="S5">
-        <f>ROUND(_xlfn.STDEV.S(M5,M5:Q5),2)</f>
+        <f t="shared" si="3"/>
         <v>0.03</v>
       </c>
     </row>
@@ -2724,11 +2731,11 @@
         <v>0.8</v>
       </c>
       <c r="G6">
-        <f>ROUND(AVERAGE(B6:F6),2)</f>
+        <f t="shared" si="0"/>
         <v>0.79</v>
       </c>
       <c r="H6">
-        <f>ROUND(_xlfn.STDEV.S(B6,B6:F6),2)</f>
+        <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
       <c r="L6">
@@ -2750,11 +2757,11 @@
         <v>0.76</v>
       </c>
       <c r="R6">
-        <f>ROUND(AVERAGE(M6:Q6),2)</f>
+        <f t="shared" si="2"/>
         <v>0.76</v>
       </c>
       <c r="S6">
-        <f>ROUND(_xlfn.STDEV.S(M6,M6:Q6),2)</f>
+        <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
     </row>
@@ -2778,11 +2785,11 @@
         <v>0.77</v>
       </c>
       <c r="G7">
-        <f>ROUND(AVERAGE(B7:F7),2)</f>
+        <f t="shared" si="0"/>
         <v>0.78</v>
       </c>
       <c r="H7">
-        <f>ROUND(_xlfn.STDEV.S(B7,B7:F7),2)</f>
+        <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
       <c r="L7">
@@ -2804,11 +2811,11 @@
         <v>0.79</v>
       </c>
       <c r="R7">
-        <f>ROUND(AVERAGE(M7:Q7),2)</f>
+        <f t="shared" si="2"/>
         <v>0.78</v>
       </c>
       <c r="S7">
-        <f>ROUND(_xlfn.STDEV.S(M7,M7:Q7),2)</f>
+        <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
     </row>
@@ -2832,11 +2839,11 @@
         <v>0.74</v>
       </c>
       <c r="G8">
-        <f>ROUND(AVERAGE(B8:F8),2)</f>
+        <f t="shared" si="0"/>
         <v>0.79</v>
       </c>
       <c r="H8">
-        <f>ROUND(_xlfn.STDEV.S(B8,B8:F8),2)</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="L8">
@@ -2858,11 +2865,11 @@
         <v>0.71</v>
       </c>
       <c r="R8">
-        <f>ROUND(AVERAGE(M8:Q8),2)</f>
+        <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
       <c r="S8">
-        <f>ROUND(_xlfn.STDEV.S(M8,M8:Q8),2)</f>
+        <f t="shared" si="3"/>
         <v>0.06</v>
       </c>
     </row>
@@ -2886,11 +2893,11 @@
         <v>0.79</v>
       </c>
       <c r="G9">
-        <f>ROUND(AVERAGE(B9:F9),2)</f>
+        <f t="shared" si="0"/>
         <v>0.73</v>
       </c>
       <c r="H9">
-        <f>ROUND(_xlfn.STDEV.S(B9,B9:F9),2)</f>
+        <f t="shared" si="1"/>
         <v>0.11</v>
       </c>
       <c r="L9">
@@ -2912,11 +2919,11 @@
         <v>0.77</v>
       </c>
       <c r="R9">
-        <f>ROUND(AVERAGE(M9:Q9),2)</f>
+        <f t="shared" si="2"/>
         <v>0.77</v>
       </c>
       <c r="S9">
-        <f>ROUND(_xlfn.STDEV.S(M9,M9:Q9),2)</f>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
     </row>
@@ -2940,11 +2947,11 @@
         <v>0.81</v>
       </c>
       <c r="G10">
-        <f>ROUND(AVERAGE(B10:F10),2)</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="H10">
-        <f>ROUND(_xlfn.STDEV.S(B10,B10:F10),2)</f>
+        <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
       <c r="L10">
@@ -2966,11 +2973,11 @@
         <v>0.77</v>
       </c>
       <c r="R10">
-        <f>ROUND(AVERAGE(M10:Q10),2)</f>
+        <f t="shared" si="2"/>
         <v>0.78</v>
       </c>
       <c r="S10">
-        <f>ROUND(_xlfn.STDEV.S(M10,M10:Q10),2)</f>
+        <f t="shared" si="3"/>
         <v>0.03</v>
       </c>
     </row>
@@ -2994,11 +3001,11 @@
         <v>0.8</v>
       </c>
       <c r="G11">
-        <f>ROUND(AVERAGE(B11:F11),2)</f>
+        <f t="shared" si="0"/>
         <v>0.78</v>
       </c>
       <c r="H11">
-        <f>ROUND(_xlfn.STDEV.S(B11,B11:F11),2)</f>
+        <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
       <c r="L11">
@@ -3020,11 +3027,11 @@
         <v>0.77</v>
       </c>
       <c r="R11">
-        <f>ROUND(AVERAGE(M11:Q11),2)</f>
+        <f t="shared" si="2"/>
         <v>0.77</v>
       </c>
       <c r="S11">
-        <f>ROUND(_xlfn.STDEV.S(M11,M11:Q11),2)</f>
+        <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
     </row>
@@ -3048,11 +3055,11 @@
         <v>0.96</v>
       </c>
       <c r="G12">
-        <f>ROUND(AVERAGE(B12:F12),2)</f>
+        <f t="shared" si="0"/>
         <v>0.83</v>
       </c>
       <c r="H12">
-        <f>ROUND(_xlfn.STDEV.S(B12,B12:F12),2)</f>
+        <f t="shared" si="1"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L12">
@@ -3074,11 +3081,11 @@
         <v>0.96</v>
       </c>
       <c r="R12">
-        <f>ROUND(AVERAGE(M12:Q12),2)</f>
+        <f t="shared" si="2"/>
         <v>0.82</v>
       </c>
       <c r="S12">
-        <f>ROUND(_xlfn.STDEV.S(M12,M12:Q12),2)</f>
+        <f t="shared" si="3"/>
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
@@ -3102,11 +3109,11 @@
         <v>0.84</v>
       </c>
       <c r="G13">
-        <f>ROUND(AVERAGE(B13:F13),2)</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="H13">
-        <f>ROUND(_xlfn.STDEV.S(B13,B13:F13),2)</f>
+        <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
       <c r="L13">
@@ -3128,11 +3135,11 @@
         <v>0.85</v>
       </c>
       <c r="R13">
-        <f>ROUND(AVERAGE(M13:Q13),2)</f>
+        <f t="shared" si="2"/>
         <v>0.79</v>
       </c>
       <c r="S13">
-        <f>ROUND(_xlfn.STDEV.S(M13,M13:Q13),2)</f>
+        <f t="shared" si="3"/>
         <v>0.04</v>
       </c>
     </row>
@@ -3156,11 +3163,11 @@
         <v>0.84</v>
       </c>
       <c r="G14">
-        <f>ROUND(AVERAGE(B14:F14),2)</f>
+        <f t="shared" si="0"/>
         <v>0.81</v>
       </c>
       <c r="H14">
-        <f>ROUND(_xlfn.STDEV.S(B14,B14:F14),2)</f>
+        <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
       <c r="L14">
@@ -3182,11 +3189,11 @@
         <v>0.8</v>
       </c>
       <c r="R14">
-        <f>ROUND(AVERAGE(M14:Q14),2)</f>
+        <f t="shared" si="2"/>
         <v>0.78</v>
       </c>
       <c r="S14">
-        <f>ROUND(_xlfn.STDEV.S(M14,M14:Q14),2)</f>
+        <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
     </row>
@@ -3210,11 +3217,11 @@
         <v>0.78</v>
       </c>
       <c r="G15">
-        <f>ROUND(AVERAGE(B15:F15),2)</f>
+        <f t="shared" si="0"/>
         <v>0.81</v>
       </c>
       <c r="H15">
-        <f>ROUND(_xlfn.STDEV.S(B15,B15:F15),2)</f>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="L15">
@@ -3236,11 +3243,11 @@
         <v>0.75</v>
       </c>
       <c r="R15">
-        <f>ROUND(AVERAGE(M15:Q15),2)</f>
+        <f t="shared" si="2"/>
         <v>0.78</v>
       </c>
       <c r="S15">
-        <f>ROUND(_xlfn.STDEV.S(M15,M15:Q15),2)</f>
+        <f t="shared" si="3"/>
         <v>0.06</v>
       </c>
     </row>
@@ -3350,37 +3357,37 @@
       <c r="R18" s="1"/>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
       <c r="I20" s="2"/>
-      <c r="L20" s="3" t="s">
+      <c r="L20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="W20" s="3" t="s">
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="W20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
-      <c r="AA20" s="3"/>
-      <c r="AB20" s="3"/>
-      <c r="AC20" s="3"/>
-      <c r="AD20" s="3"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="6"/>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="6"/>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -3476,11 +3483,11 @@
         <v>0.75</v>
       </c>
       <c r="G22">
-        <f>ROUND(AVERAGE(B22:F22),2)</f>
+        <f t="shared" ref="G22:G33" si="4">ROUND(AVERAGE(B22:F22),2)</f>
         <v>0.73</v>
       </c>
       <c r="H22">
-        <f>ROUND(_xlfn.STDEV.S(B22,B22:F22),2)</f>
+        <f t="shared" ref="H22:H33" si="5">ROUND(_xlfn.STDEV.S(B22,B22:F22),2)</f>
         <v>0.06</v>
       </c>
       <c r="L22">
@@ -3502,11 +3509,11 @@
         <v>0.8</v>
       </c>
       <c r="R22">
-        <f>ROUND(AVERAGE(M22:Q22),2)</f>
+        <f t="shared" ref="R22:R33" si="6">ROUND(AVERAGE(M22:Q22),2)</f>
         <v>0.81</v>
       </c>
       <c r="S22">
-        <f>ROUND(_xlfn.STDEV.S(M22,M22:Q22),2)</f>
+        <f t="shared" ref="S22:S33" si="7">ROUND(_xlfn.STDEV.S(M22,M22:Q22),2)</f>
         <v>0.03</v>
       </c>
       <c r="W22">
@@ -3528,11 +3535,11 @@
         <v>0.75</v>
       </c>
       <c r="AC22">
-        <f>ROUND(AVERAGE(X22:AB22),2)</f>
+        <f t="shared" ref="AC22:AC33" si="8">ROUND(AVERAGE(X22:AB22),2)</f>
         <v>0.78</v>
       </c>
       <c r="AD22">
-        <f>ROUND(_xlfn.STDEV.S(X22,X22:AB22),2)</f>
+        <f t="shared" ref="AD22:AD33" si="9">ROUND(_xlfn.STDEV.S(X22,X22:AB22),2)</f>
         <v>0.04</v>
       </c>
     </row>
@@ -3556,11 +3563,11 @@
         <v>0.68</v>
       </c>
       <c r="G23">
-        <f>ROUND(AVERAGE(B23:F23),2)</f>
+        <f t="shared" si="4"/>
         <v>0.77</v>
       </c>
       <c r="H23">
-        <f>ROUND(_xlfn.STDEV.S(B23,B23:F23),2)</f>
+        <f t="shared" si="5"/>
         <v>0.06</v>
       </c>
       <c r="L23">
@@ -3582,11 +3589,11 @@
         <v>0.79</v>
       </c>
       <c r="R23">
-        <f>ROUND(AVERAGE(M23:Q23),2)</f>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="S23">
-        <f>ROUND(_xlfn.STDEV.S(M23,M23:Q23),2)</f>
+        <f t="shared" si="7"/>
         <v>0.02</v>
       </c>
       <c r="W23">
@@ -3608,11 +3615,11 @@
         <v>0.74</v>
       </c>
       <c r="AC23">
-        <f>ROUND(AVERAGE(X23:AB23),2)</f>
+        <f t="shared" si="8"/>
         <v>0.77</v>
       </c>
       <c r="AD23">
-        <f>ROUND(_xlfn.STDEV.S(X23,X23:AB23),2)</f>
+        <f t="shared" si="9"/>
         <v>0.03</v>
       </c>
     </row>
@@ -3636,11 +3643,11 @@
         <v>0.78</v>
       </c>
       <c r="G24">
-        <f>ROUND(AVERAGE(B24:F24),2)</f>
+        <f t="shared" si="4"/>
         <v>0.75</v>
       </c>
       <c r="H24">
-        <f>ROUND(_xlfn.STDEV.S(B24,B24:F24),2)</f>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="L24">
@@ -3662,11 +3669,11 @@
         <v>0.81</v>
       </c>
       <c r="R24">
-        <f>ROUND(AVERAGE(M24:Q24),2)</f>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="S24">
-        <f>ROUND(_xlfn.STDEV.S(M24,M24:Q24),2)</f>
+        <f t="shared" si="7"/>
         <v>0.02</v>
       </c>
       <c r="W24">
@@ -3688,11 +3695,11 @@
         <v>0.76</v>
       </c>
       <c r="AC24">
-        <f>ROUND(AVERAGE(X24:AB24),2)</f>
+        <f t="shared" si="8"/>
         <v>0.76</v>
       </c>
       <c r="AD24">
-        <f>ROUND(_xlfn.STDEV.S(X24,X24:AB24),2)</f>
+        <f t="shared" si="9"/>
         <v>0.02</v>
       </c>
     </row>
@@ -3716,11 +3723,11 @@
         <v>0.67</v>
       </c>
       <c r="G25">
-        <f>ROUND(AVERAGE(B25:F25),2)</f>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="H25">
-        <f>ROUND(_xlfn.STDEV.S(B25,B25:F25),2)</f>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="L25">
@@ -3742,11 +3749,11 @@
         <v>0.8</v>
       </c>
       <c r="R25">
-        <f>ROUND(AVERAGE(M25:Q25),2)</f>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="S25">
-        <f>ROUND(_xlfn.STDEV.S(M25,M25:Q25),2)</f>
+        <f t="shared" si="7"/>
         <v>0.01</v>
       </c>
       <c r="W25">
@@ -3768,11 +3775,11 @@
         <v>0.79</v>
       </c>
       <c r="AC25">
-        <f>ROUND(AVERAGE(X25:AB25),2)</f>
+        <f t="shared" si="8"/>
         <v>0.78</v>
       </c>
       <c r="AD25">
-        <f>ROUND(_xlfn.STDEV.S(X25,X25:AB25),2)</f>
+        <f t="shared" si="9"/>
         <v>0.01</v>
       </c>
     </row>
@@ -3796,11 +3803,11 @@
         <v>0.65</v>
       </c>
       <c r="G26">
-        <f>ROUND(AVERAGE(B26:F26),2)</f>
+        <f t="shared" si="4"/>
         <v>0.67</v>
       </c>
       <c r="H26">
-        <f>ROUND(_xlfn.STDEV.S(B26,B26:F26),2)</f>
+        <f t="shared" si="5"/>
         <v>0.02</v>
       </c>
       <c r="L26">
@@ -3822,11 +3829,11 @@
         <v>0.78</v>
       </c>
       <c r="R26">
-        <f>ROUND(AVERAGE(M26:Q26),2)</f>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="S26">
-        <f>ROUND(_xlfn.STDEV.S(M26,M26:Q26),2)</f>
+        <f t="shared" si="7"/>
         <v>0.03</v>
       </c>
       <c r="W26">
@@ -3848,11 +3855,11 @@
         <v>0.71</v>
       </c>
       <c r="AC26">
-        <f>ROUND(AVERAGE(X26:AB26),2)</f>
+        <f t="shared" si="8"/>
         <v>0.75</v>
       </c>
       <c r="AD26">
-        <f>ROUND(_xlfn.STDEV.S(X26,X26:AB26),2)</f>
+        <f t="shared" si="9"/>
         <v>0.06</v>
       </c>
     </row>
@@ -3876,11 +3883,11 @@
         <v>0.74</v>
       </c>
       <c r="G27">
-        <f>ROUND(AVERAGE(B27:F27),2)</f>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="H27">
-        <f>ROUND(_xlfn.STDEV.S(B27,B27:F27),2)</f>
+        <f t="shared" si="5"/>
         <v>0.09</v>
       </c>
       <c r="L27">
@@ -3902,11 +3909,11 @@
         <v>0.78</v>
       </c>
       <c r="R27">
-        <f>ROUND(AVERAGE(M27:Q27),2)</f>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="S27">
-        <f>ROUND(_xlfn.STDEV.S(M27,M27:Q27),2)</f>
+        <f t="shared" si="7"/>
         <v>0.03</v>
       </c>
       <c r="W27">
@@ -3928,11 +3935,11 @@
         <v>0.77</v>
       </c>
       <c r="AC27">
-        <f>ROUND(AVERAGE(X27:AB27),2)</f>
+        <f t="shared" si="8"/>
         <v>0.77</v>
       </c>
       <c r="AD27">
-        <f>ROUND(_xlfn.STDEV.S(X27,X27:AB27),2)</f>
+        <f t="shared" si="9"/>
         <v>0.05</v>
       </c>
     </row>
@@ -3956,11 +3963,11 @@
         <v>0.75</v>
       </c>
       <c r="G28">
-        <f>ROUND(AVERAGE(B28:F28),2)</f>
+        <f t="shared" si="4"/>
         <v>0.72</v>
       </c>
       <c r="H28">
-        <f>ROUND(_xlfn.STDEV.S(B28,B28:F28),2)</f>
+        <f t="shared" si="5"/>
         <v>0.05</v>
       </c>
       <c r="L28">
@@ -3982,11 +3989,11 @@
         <v>0.8</v>
       </c>
       <c r="R28">
-        <f>ROUND(AVERAGE(M28:Q28),2)</f>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="S28">
-        <f>ROUND(_xlfn.STDEV.S(M28,M28:Q28),2)</f>
+        <f t="shared" si="7"/>
         <v>0.02</v>
       </c>
       <c r="W28">
@@ -4008,11 +4015,11 @@
         <v>0.77</v>
       </c>
       <c r="AC28">
-        <f>ROUND(AVERAGE(X28:AB28),2)</f>
+        <f t="shared" si="8"/>
         <v>0.78</v>
       </c>
       <c r="AD28">
-        <f>ROUND(_xlfn.STDEV.S(X28,X28:AB28),2)</f>
+        <f t="shared" si="9"/>
         <v>0.03</v>
       </c>
     </row>
@@ -4036,11 +4043,11 @@
         <v>0.68</v>
       </c>
       <c r="G29">
-        <f>ROUND(AVERAGE(B29:F29),2)</f>
+        <f t="shared" si="4"/>
         <v>0.69</v>
       </c>
       <c r="H29">
-        <f>ROUND(_xlfn.STDEV.S(B29,B29:F29),2)</f>
+        <f t="shared" si="5"/>
         <v>0.02</v>
       </c>
       <c r="L29">
@@ -4062,11 +4069,11 @@
         <v>0.8</v>
       </c>
       <c r="R29">
-        <f>ROUND(AVERAGE(M29:Q29),2)</f>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="S29">
-        <f>ROUND(_xlfn.STDEV.S(M29,M29:Q29),2)</f>
+        <f t="shared" si="7"/>
         <v>0.01</v>
       </c>
       <c r="W29">
@@ -4088,11 +4095,11 @@
         <v>0.77</v>
       </c>
       <c r="AC29">
-        <f>ROUND(AVERAGE(X29:AB29),2)</f>
+        <f t="shared" si="8"/>
         <v>0.77</v>
       </c>
       <c r="AD29">
-        <f>ROUND(_xlfn.STDEV.S(X29,X29:AB29),2)</f>
+        <f t="shared" si="9"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4116,11 +4123,11 @@
         <v>0.94</v>
       </c>
       <c r="G30">
-        <f>ROUND(AVERAGE(B30:F30),2)</f>
+        <f t="shared" si="4"/>
         <v>0.76</v>
       </c>
       <c r="H30">
-        <f>ROUND(_xlfn.STDEV.S(B30,B30:F30),2)</f>
+        <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
       <c r="L30">
@@ -4142,11 +4149,11 @@
         <v>0.96</v>
       </c>
       <c r="R30">
-        <f>ROUND(AVERAGE(M30:Q30),2)</f>
+        <f t="shared" si="6"/>
         <v>0.84</v>
       </c>
       <c r="S30">
-        <f>ROUND(_xlfn.STDEV.S(M30,M30:Q30),2)</f>
+        <f t="shared" si="7"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="W30">
@@ -4168,11 +4175,11 @@
         <v>0.96</v>
       </c>
       <c r="AC30">
-        <f>ROUND(AVERAGE(X30:AB30),2)</f>
+        <f t="shared" si="8"/>
         <v>0.82</v>
       </c>
       <c r="AD30">
-        <f>ROUND(_xlfn.STDEV.S(X30,X30:AB30),2)</f>
+        <f t="shared" si="9"/>
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
@@ -4196,11 +4203,11 @@
         <v>0.76</v>
       </c>
       <c r="G31">
-        <f>ROUND(AVERAGE(B31:F31),2)</f>
+        <f t="shared" si="4"/>
         <v>0.72</v>
       </c>
       <c r="H31">
-        <f>ROUND(_xlfn.STDEV.S(B31,B31:F31),2)</f>
+        <f t="shared" si="5"/>
         <v>0.03</v>
       </c>
       <c r="L31">
@@ -4222,11 +4229,11 @@
         <v>0.81</v>
       </c>
       <c r="R31">
-        <f>ROUND(AVERAGE(M31:Q31),2)</f>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="S31">
-        <f>ROUND(_xlfn.STDEV.S(M31,M31:Q31),2)</f>
+        <f t="shared" si="7"/>
         <v>0.01</v>
       </c>
       <c r="W31">
@@ -4248,11 +4255,11 @@
         <v>0.85</v>
       </c>
       <c r="AC31">
-        <f>ROUND(AVERAGE(X31:AB31),2)</f>
+        <f t="shared" si="8"/>
         <v>0.79</v>
       </c>
       <c r="AD31">
-        <f>ROUND(_xlfn.STDEV.S(X31,X31:AB31),2)</f>
+        <f t="shared" si="9"/>
         <v>0.04</v>
       </c>
     </row>
@@ -4276,11 +4283,11 @@
         <v>0.81</v>
       </c>
       <c r="G32">
-        <f>ROUND(AVERAGE(B32:F32),2)</f>
+        <f t="shared" si="4"/>
         <v>0.74</v>
       </c>
       <c r="H32">
-        <f>ROUND(_xlfn.STDEV.S(B32,B32:F32),2)</f>
+        <f t="shared" si="5"/>
         <v>0.05</v>
       </c>
       <c r="L32">
@@ -4302,11 +4309,11 @@
         <v>0.8</v>
       </c>
       <c r="R32">
-        <f>ROUND(AVERAGE(M32:Q32),2)</f>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="S32">
-        <f>ROUND(_xlfn.STDEV.S(M32,M32:Q32),2)</f>
+        <f t="shared" si="7"/>
         <v>0.01</v>
       </c>
       <c r="W32">
@@ -4328,11 +4335,11 @@
         <v>0.8</v>
       </c>
       <c r="AC32">
-        <f>ROUND(AVERAGE(X32:AB32),2)</f>
+        <f t="shared" si="8"/>
         <v>0.78</v>
       </c>
       <c r="AD32">
-        <f>ROUND(_xlfn.STDEV.S(X32,X32:AB32),2)</f>
+        <f t="shared" si="9"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4356,11 +4363,11 @@
         <v>0.68</v>
       </c>
       <c r="G33">
-        <f>ROUND(AVERAGE(B33:F33),2)</f>
+        <f t="shared" si="4"/>
         <v>0.76</v>
       </c>
       <c r="H33">
-        <f>ROUND(_xlfn.STDEV.S(B33,B33:F33),2)</f>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L33">
@@ -4382,11 +4389,11 @@
         <v>0.8</v>
       </c>
       <c r="R33">
-        <f>ROUND(AVERAGE(M33:Q33),2)</f>
+        <f t="shared" si="6"/>
         <v>0.81</v>
       </c>
       <c r="S33">
-        <f>ROUND(_xlfn.STDEV.S(M33,M33:Q33),2)</f>
+        <f t="shared" si="7"/>
         <v>0.02</v>
       </c>
       <c r="W33">
@@ -4408,11 +4415,11 @@
         <v>0.75</v>
       </c>
       <c r="AC33">
-        <f>ROUND(AVERAGE(X33:AB33),2)</f>
+        <f t="shared" si="8"/>
         <v>0.78</v>
       </c>
       <c r="AD33">
-        <f>ROUND(_xlfn.STDEV.S(X33,X33:AB33),2)</f>
+        <f t="shared" si="9"/>
         <v>0.06</v>
       </c>
     </row>
@@ -4556,6 +4563,41 @@
       <c r="AB35" s="1">
         <f>ROUND(_xlfn.STDEV.S(AB22:AB33),2)</f>
         <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36">
+        <f>MAX(B22:F33)</f>
+        <v>0.94</v>
+      </c>
+      <c r="C36">
+        <f>MIN(B22:F33)</f>
+        <v>0.59</v>
+      </c>
+      <c r="L36" t="s">
+        <v>21</v>
+      </c>
+      <c r="M36">
+        <f>MAX(M22:Q33)</f>
+        <v>0.96</v>
+      </c>
+      <c r="N36">
+        <f>MIN(M22:Q33)</f>
+        <v>0.77</v>
+      </c>
+      <c r="W36" t="s">
+        <v>21</v>
+      </c>
+      <c r="X36">
+        <f>MAX(X22:AB33)</f>
+        <v>0.96</v>
+      </c>
+      <c r="Y36">
+        <f>MIN(X22:AB33)</f>
+        <v>0.67</v>
       </c>
     </row>
   </sheetData>
@@ -4569,4 +4611,1691 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF67C51-784B-4AA6-B43B-1BF7650FC051}">
+  <dimension ref="A1:AD35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G15" workbookViewId="0">
+      <selection activeCell="AA42" sqref="AA42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:20" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="3"/>
+      <c r="L2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="4"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R3" t="s">
+        <v>7</v>
+      </c>
+      <c r="S3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0.8</v>
+      </c>
+      <c r="C4">
+        <v>0.78</v>
+      </c>
+      <c r="D4">
+        <v>0.79</v>
+      </c>
+      <c r="E4">
+        <v>0.83</v>
+      </c>
+      <c r="F4">
+        <v>0.82</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G15" si="0">ROUND(AVERAGE(B4:F4),2)</f>
+        <v>0.8</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H15" si="1">ROUND(_xlfn.STDEV.S(B4,B4:F4),2)</f>
+        <v>0.02</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0.76</v>
+      </c>
+      <c r="N4">
+        <v>0.76</v>
+      </c>
+      <c r="O4">
+        <v>0.79</v>
+      </c>
+      <c r="P4">
+        <v>0.86</v>
+      </c>
+      <c r="Q4">
+        <v>0.75</v>
+      </c>
+      <c r="R4">
+        <f t="shared" ref="R4:R15" si="2">ROUND(AVERAGE(M4:Q4),2)</f>
+        <v>0.78</v>
+      </c>
+      <c r="S4">
+        <f t="shared" ref="S4:S15" si="3">ROUND(_xlfn.STDEV.S(M4,M4:Q4),2)</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0.8</v>
+      </c>
+      <c r="C5">
+        <v>0.87</v>
+      </c>
+      <c r="D5">
+        <v>0.82</v>
+      </c>
+      <c r="E5">
+        <v>0.81</v>
+      </c>
+      <c r="F5">
+        <v>0.76</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>0.81</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>0.04</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>0.79</v>
+      </c>
+      <c r="N5">
+        <v>0.79</v>
+      </c>
+      <c r="O5">
+        <v>0.78</v>
+      </c>
+      <c r="P5">
+        <v>0.73</v>
+      </c>
+      <c r="Q5">
+        <v>0.74</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="2"/>
+        <v>0.77</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="3"/>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>0.78</v>
+      </c>
+      <c r="C6">
+        <v>0.75</v>
+      </c>
+      <c r="D6">
+        <v>0.83</v>
+      </c>
+      <c r="E6">
+        <v>0.79</v>
+      </c>
+      <c r="F6">
+        <v>0.8</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>0.79</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>0.03</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6">
+        <v>0.76</v>
+      </c>
+      <c r="N6">
+        <v>0.73</v>
+      </c>
+      <c r="O6">
+        <v>0.79</v>
+      </c>
+      <c r="P6">
+        <v>0.78</v>
+      </c>
+      <c r="Q6">
+        <v>0.76</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="2"/>
+        <v>0.76</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="3"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>0.74</v>
+      </c>
+      <c r="C7">
+        <v>0.83</v>
+      </c>
+      <c r="D7">
+        <v>0.79</v>
+      </c>
+      <c r="E7">
+        <v>0.79</v>
+      </c>
+      <c r="F7">
+        <v>0.77</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.78</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>0.03</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <v>0.76</v>
+      </c>
+      <c r="N7">
+        <v>0.77</v>
+      </c>
+      <c r="O7">
+        <v>0.77</v>
+      </c>
+      <c r="P7">
+        <v>0.79</v>
+      </c>
+      <c r="Q7">
+        <v>0.79</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="2"/>
+        <v>0.78</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="3"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>0.73</v>
+      </c>
+      <c r="C8">
+        <v>0.82</v>
+      </c>
+      <c r="D8">
+        <v>0.8</v>
+      </c>
+      <c r="E8">
+        <v>0.85</v>
+      </c>
+      <c r="F8">
+        <v>0.74</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0.79</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+      <c r="M8">
+        <v>0.67</v>
+      </c>
+      <c r="N8">
+        <v>0.76</v>
+      </c>
+      <c r="O8">
+        <v>0.77</v>
+      </c>
+      <c r="P8">
+        <v>0.82</v>
+      </c>
+      <c r="Q8">
+        <v>0.71</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="3"/>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>0.78</v>
+      </c>
+      <c r="C9">
+        <v>0.61</v>
+      </c>
+      <c r="D9">
+        <v>0.6</v>
+      </c>
+      <c r="E9">
+        <v>0.88</v>
+      </c>
+      <c r="F9">
+        <v>0.79</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0.73</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>0.11</v>
+      </c>
+      <c r="L9">
+        <v>6</v>
+      </c>
+      <c r="M9">
+        <v>0.77</v>
+      </c>
+      <c r="N9">
+        <v>0.72</v>
+      </c>
+      <c r="O9">
+        <v>0.74</v>
+      </c>
+      <c r="P9">
+        <v>0.86</v>
+      </c>
+      <c r="Q9">
+        <v>0.77</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="2"/>
+        <v>0.77</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>0.79</v>
+      </c>
+      <c r="C10">
+        <v>0.78</v>
+      </c>
+      <c r="D10">
+        <v>0.82</v>
+      </c>
+      <c r="E10">
+        <v>0.78</v>
+      </c>
+      <c r="F10">
+        <v>0.81</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="L10">
+        <v>7</v>
+      </c>
+      <c r="M10">
+        <v>0.76</v>
+      </c>
+      <c r="N10">
+        <v>0.75</v>
+      </c>
+      <c r="O10">
+        <v>0.83</v>
+      </c>
+      <c r="P10">
+        <v>0.77</v>
+      </c>
+      <c r="Q10">
+        <v>0.77</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="2"/>
+        <v>0.78</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="3"/>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0.77</v>
+      </c>
+      <c r="C11">
+        <v>0.76</v>
+      </c>
+      <c r="D11">
+        <v>0.79</v>
+      </c>
+      <c r="E11">
+        <v>0.79</v>
+      </c>
+      <c r="F11">
+        <v>0.8</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0.78</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="L11">
+        <v>8</v>
+      </c>
+      <c r="M11">
+        <v>0.77</v>
+      </c>
+      <c r="N11">
+        <v>0.74</v>
+      </c>
+      <c r="O11">
+        <v>0.8</v>
+      </c>
+      <c r="P11">
+        <v>0.77</v>
+      </c>
+      <c r="Q11">
+        <v>0.77</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="2"/>
+        <v>0.77</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="3"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>0.79</v>
+      </c>
+      <c r="C12">
+        <v>0.83</v>
+      </c>
+      <c r="D12">
+        <v>0.75</v>
+      </c>
+      <c r="E12">
+        <v>0.81</v>
+      </c>
+      <c r="F12">
+        <v>0.96</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0.83</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L12">
+        <v>9</v>
+      </c>
+      <c r="M12">
+        <v>0.81</v>
+      </c>
+      <c r="N12">
+        <v>0.79</v>
+      </c>
+      <c r="O12">
+        <v>0.75</v>
+      </c>
+      <c r="P12">
+        <v>0.78</v>
+      </c>
+      <c r="Q12">
+        <v>0.96</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="2"/>
+        <v>0.82</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="3"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>0.8</v>
+      </c>
+      <c r="C13">
+        <v>0.77</v>
+      </c>
+      <c r="D13">
+        <v>0.79</v>
+      </c>
+      <c r="E13">
+        <v>0.79</v>
+      </c>
+      <c r="F13">
+        <v>0.84</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="L13">
+        <v>10</v>
+      </c>
+      <c r="M13">
+        <v>0.8</v>
+      </c>
+      <c r="N13">
+        <v>0.74</v>
+      </c>
+      <c r="O13">
+        <v>0.77</v>
+      </c>
+      <c r="P13">
+        <v>0.78</v>
+      </c>
+      <c r="Q13">
+        <v>0.85</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="2"/>
+        <v>0.79</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>0.8</v>
+      </c>
+      <c r="C14">
+        <v>0.81</v>
+      </c>
+      <c r="D14">
+        <v>0.79</v>
+      </c>
+      <c r="E14">
+        <v>0.8</v>
+      </c>
+      <c r="F14">
+        <v>0.84</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0.81</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="L14">
+        <v>11</v>
+      </c>
+      <c r="M14">
+        <v>0.76</v>
+      </c>
+      <c r="N14">
+        <v>0.79</v>
+      </c>
+      <c r="O14">
+        <v>0.79</v>
+      </c>
+      <c r="P14">
+        <v>0.75</v>
+      </c>
+      <c r="Q14">
+        <v>0.8</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="2"/>
+        <v>0.78</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="3"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>0.79</v>
+      </c>
+      <c r="C15">
+        <v>0.81</v>
+      </c>
+      <c r="D15">
+        <v>0.79</v>
+      </c>
+      <c r="E15">
+        <v>0.88</v>
+      </c>
+      <c r="F15">
+        <v>0.78</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0.81</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>0.04</v>
+      </c>
+      <c r="L15">
+        <v>12</v>
+      </c>
+      <c r="M15">
+        <v>0.75</v>
+      </c>
+      <c r="N15">
+        <v>0.77</v>
+      </c>
+      <c r="O15">
+        <v>0.76</v>
+      </c>
+      <c r="P15">
+        <v>0.89</v>
+      </c>
+      <c r="Q15">
+        <v>0.75</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="2"/>
+        <v>0.78</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="3"/>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <f>ROUND(AVERAGE(B4:B15),2)</f>
+        <v>0.78</v>
+      </c>
+      <c r="C16">
+        <f>ROUND(AVERAGE(C4:C15),2)</f>
+        <v>0.79</v>
+      </c>
+      <c r="D16">
+        <f>ROUND(AVERAGE(D4:D15),2)</f>
+        <v>0.78</v>
+      </c>
+      <c r="E16">
+        <f>ROUND(AVERAGE(E4:E15),2)</f>
+        <v>0.82</v>
+      </c>
+      <c r="F16">
+        <f>ROUND(AVERAGE(F4:F15),2)</f>
+        <v>0.81</v>
+      </c>
+      <c r="L16" t="s">
+        <v>7</v>
+      </c>
+      <c r="M16">
+        <f>ROUND(AVERAGE(M4:M15),2)</f>
+        <v>0.76</v>
+      </c>
+      <c r="N16">
+        <f>ROUND(AVERAGE(N4:N15),2)</f>
+        <v>0.76</v>
+      </c>
+      <c r="O16">
+        <f>ROUND(AVERAGE(O4:O15),2)</f>
+        <v>0.78</v>
+      </c>
+      <c r="P16">
+        <f>ROUND(AVERAGE(P4:P15),2)</f>
+        <v>0.8</v>
+      </c>
+      <c r="Q16">
+        <f>ROUND(AVERAGE(Q4:Q15),2)</f>
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1">
+        <f>ROUND(_xlfn.STDEV.S(B4:B15),2)</f>
+        <v>0.02</v>
+      </c>
+      <c r="C17" s="1">
+        <f>ROUND(_xlfn.STDEV.S(C4:C15),2)</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D17" s="1">
+        <f>ROUND(_xlfn.STDEV.S(D4:D15),2)</f>
+        <v>0.06</v>
+      </c>
+      <c r="E17" s="1">
+        <f>ROUND(_xlfn.STDEV.S(E4:E15),2)</f>
+        <v>0.04</v>
+      </c>
+      <c r="F17" s="1">
+        <f>ROUND(_xlfn.STDEV.S(F4:F15),2)</f>
+        <v>0.06</v>
+      </c>
+      <c r="L17" t="s">
+        <v>8</v>
+      </c>
+      <c r="M17" s="1">
+        <f>ROUND(_xlfn.STDEV.S(M4:M15),2)</f>
+        <v>0.03</v>
+      </c>
+      <c r="N17" s="1">
+        <f>ROUND(_xlfn.STDEV.S(N4:N15),2)</f>
+        <v>0.02</v>
+      </c>
+      <c r="O17" s="1">
+        <f>ROUND(_xlfn.STDEV.S(O4:O15),2)</f>
+        <v>0.02</v>
+      </c>
+      <c r="P17" s="1">
+        <f>ROUND(_xlfn.STDEV.S(P4:P15),2)</f>
+        <v>0.05</v>
+      </c>
+      <c r="Q17" s="1">
+        <f>ROUND(_xlfn.STDEV.S(Q4:Q15),2)</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="G18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="3"/>
+      <c r="L20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="W20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="6"/>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="6"/>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" t="s">
+        <v>18</v>
+      </c>
+      <c r="L21" t="s">
+        <v>2</v>
+      </c>
+      <c r="M21" t="s">
+        <v>14</v>
+      </c>
+      <c r="N21" t="s">
+        <v>15</v>
+      </c>
+      <c r="O21" t="s">
+        <v>16</v>
+      </c>
+      <c r="P21" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>18</v>
+      </c>
+      <c r="W21" t="s">
+        <v>2</v>
+      </c>
+      <c r="X21" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>0.73</v>
+      </c>
+      <c r="C22">
+        <v>0.66</v>
+      </c>
+      <c r="D22">
+        <v>0.69</v>
+      </c>
+      <c r="E22">
+        <v>0.83</v>
+      </c>
+      <c r="F22">
+        <v>0.75</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>0.79</v>
+      </c>
+      <c r="N22">
+        <v>0.79</v>
+      </c>
+      <c r="O22">
+        <v>0.79</v>
+      </c>
+      <c r="P22">
+        <v>0.86</v>
+      </c>
+      <c r="Q22">
+        <v>0.8</v>
+      </c>
+      <c r="W22">
+        <v>1</v>
+      </c>
+      <c r="X22">
+        <v>0.76</v>
+      </c>
+      <c r="Y22">
+        <v>0.76</v>
+      </c>
+      <c r="Z22">
+        <v>0.79</v>
+      </c>
+      <c r="AA22">
+        <v>0.86</v>
+      </c>
+      <c r="AB22">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>0.82</v>
+      </c>
+      <c r="C23">
+        <v>0.8</v>
+      </c>
+      <c r="D23">
+        <v>0.75</v>
+      </c>
+      <c r="E23">
+        <v>0.82</v>
+      </c>
+      <c r="F23">
+        <v>0.68</v>
+      </c>
+      <c r="L23">
+        <v>2</v>
+      </c>
+      <c r="M23">
+        <v>0.8</v>
+      </c>
+      <c r="N23">
+        <v>0.82</v>
+      </c>
+      <c r="O23">
+        <v>0.82</v>
+      </c>
+      <c r="P23">
+        <v>0.78</v>
+      </c>
+      <c r="Q23">
+        <v>0.79</v>
+      </c>
+      <c r="W23">
+        <v>2</v>
+      </c>
+      <c r="X23">
+        <v>0.79</v>
+      </c>
+      <c r="Y23">
+        <v>0.79</v>
+      </c>
+      <c r="Z23">
+        <v>0.78</v>
+      </c>
+      <c r="AA23">
+        <v>0.73</v>
+      </c>
+      <c r="AB23">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>0.7</v>
+      </c>
+      <c r="C24">
+        <v>0.76</v>
+      </c>
+      <c r="D24">
+        <v>0.77</v>
+      </c>
+      <c r="E24">
+        <v>0.72</v>
+      </c>
+      <c r="F24">
+        <v>0.78</v>
+      </c>
+      <c r="L24">
+        <v>3</v>
+      </c>
+      <c r="M24">
+        <v>0.77</v>
+      </c>
+      <c r="N24">
+        <v>0.79</v>
+      </c>
+      <c r="O24">
+        <v>0.83</v>
+      </c>
+      <c r="P24">
+        <v>0.81</v>
+      </c>
+      <c r="Q24">
+        <v>0.81</v>
+      </c>
+      <c r="W24">
+        <v>3</v>
+      </c>
+      <c r="X24">
+        <v>0.76</v>
+      </c>
+      <c r="Y24">
+        <v>0.73</v>
+      </c>
+      <c r="Z24">
+        <v>0.79</v>
+      </c>
+      <c r="AA24">
+        <v>0.78</v>
+      </c>
+      <c r="AB24">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>0.67</v>
+      </c>
+      <c r="C25">
+        <v>0.73</v>
+      </c>
+      <c r="D25">
+        <v>0.69</v>
+      </c>
+      <c r="E25">
+        <v>0.75</v>
+      </c>
+      <c r="F25">
+        <v>0.67</v>
+      </c>
+      <c r="L25">
+        <v>4</v>
+      </c>
+      <c r="M25">
+        <v>0.79</v>
+      </c>
+      <c r="N25">
+        <v>0.8</v>
+      </c>
+      <c r="O25">
+        <v>0.8</v>
+      </c>
+      <c r="P25">
+        <v>0.81</v>
+      </c>
+      <c r="Q25">
+        <v>0.8</v>
+      </c>
+      <c r="W25">
+        <v>4</v>
+      </c>
+      <c r="X25">
+        <v>0.76</v>
+      </c>
+      <c r="Y25">
+        <v>0.77</v>
+      </c>
+      <c r="Z25">
+        <v>0.77</v>
+      </c>
+      <c r="AA25">
+        <v>0.79</v>
+      </c>
+      <c r="AB25">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>0.67</v>
+      </c>
+      <c r="C26">
+        <v>0.66</v>
+      </c>
+      <c r="D26">
+        <v>0.67</v>
+      </c>
+      <c r="E26">
+        <v>0.71</v>
+      </c>
+      <c r="F26">
+        <v>0.65</v>
+      </c>
+      <c r="L26">
+        <v>5</v>
+      </c>
+      <c r="M26">
+        <v>0.77</v>
+      </c>
+      <c r="N26">
+        <v>0.82</v>
+      </c>
+      <c r="O26">
+        <v>0.79</v>
+      </c>
+      <c r="P26">
+        <v>0.85</v>
+      </c>
+      <c r="Q26">
+        <v>0.78</v>
+      </c>
+      <c r="W26">
+        <v>5</v>
+      </c>
+      <c r="X26">
+        <v>0.67</v>
+      </c>
+      <c r="Y26">
+        <v>0.76</v>
+      </c>
+      <c r="Z26">
+        <v>0.77</v>
+      </c>
+      <c r="AA26">
+        <v>0.82</v>
+      </c>
+      <c r="AB26">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>0.73</v>
+      </c>
+      <c r="C27">
+        <v>0.61</v>
+      </c>
+      <c r="D27">
+        <v>0.59</v>
+      </c>
+      <c r="E27">
+        <v>0.84</v>
+      </c>
+      <c r="F27">
+        <v>0.74</v>
+      </c>
+      <c r="L27">
+        <v>6</v>
+      </c>
+      <c r="M27">
+        <v>0.79</v>
+      </c>
+      <c r="N27">
+        <v>0.79</v>
+      </c>
+      <c r="O27">
+        <v>0.79</v>
+      </c>
+      <c r="P27">
+        <v>0.86</v>
+      </c>
+      <c r="Q27">
+        <v>0.78</v>
+      </c>
+      <c r="W27">
+        <v>6</v>
+      </c>
+      <c r="X27">
+        <v>0.77</v>
+      </c>
+      <c r="Y27">
+        <v>0.72</v>
+      </c>
+      <c r="Z27">
+        <v>0.74</v>
+      </c>
+      <c r="AA27">
+        <v>0.86</v>
+      </c>
+      <c r="AB27">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28">
+        <v>0.66</v>
+      </c>
+      <c r="C28">
+        <v>0.69</v>
+      </c>
+      <c r="D28">
+        <v>0.79</v>
+      </c>
+      <c r="E28">
+        <v>0.69</v>
+      </c>
+      <c r="F28">
+        <v>0.75</v>
+      </c>
+      <c r="L28">
+        <v>7</v>
+      </c>
+      <c r="M28">
+        <v>0.79</v>
+      </c>
+      <c r="N28">
+        <v>0.79</v>
+      </c>
+      <c r="O28">
+        <v>0.83</v>
+      </c>
+      <c r="P28">
+        <v>0.79</v>
+      </c>
+      <c r="Q28">
+        <v>0.8</v>
+      </c>
+      <c r="W28">
+        <v>7</v>
+      </c>
+      <c r="X28">
+        <v>0.76</v>
+      </c>
+      <c r="Y28">
+        <v>0.75</v>
+      </c>
+      <c r="Z28">
+        <v>0.83</v>
+      </c>
+      <c r="AA28">
+        <v>0.77</v>
+      </c>
+      <c r="AB28">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>0.67</v>
+      </c>
+      <c r="C29">
+        <v>0.68</v>
+      </c>
+      <c r="D29">
+        <v>0.7</v>
+      </c>
+      <c r="E29">
+        <v>0.71</v>
+      </c>
+      <c r="F29">
+        <v>0.68</v>
+      </c>
+      <c r="L29">
+        <v>8</v>
+      </c>
+      <c r="M29">
+        <v>0.8</v>
+      </c>
+      <c r="N29">
+        <v>0.79</v>
+      </c>
+      <c r="O29">
+        <v>0.81</v>
+      </c>
+      <c r="P29">
+        <v>0.8</v>
+      </c>
+      <c r="Q29">
+        <v>0.8</v>
+      </c>
+      <c r="W29">
+        <v>8</v>
+      </c>
+      <c r="X29">
+        <v>0.77</v>
+      </c>
+      <c r="Y29">
+        <v>0.74</v>
+      </c>
+      <c r="Z29">
+        <v>0.8</v>
+      </c>
+      <c r="AA29">
+        <v>0.77</v>
+      </c>
+      <c r="AB29">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>9</v>
+      </c>
+      <c r="B30">
+        <v>0.71</v>
+      </c>
+      <c r="C30">
+        <v>0.77</v>
+      </c>
+      <c r="D30">
+        <v>0.68</v>
+      </c>
+      <c r="E30">
+        <v>0.69</v>
+      </c>
+      <c r="F30">
+        <v>0.94</v>
+      </c>
+      <c r="L30">
+        <v>9</v>
+      </c>
+      <c r="M30">
+        <v>0.82</v>
+      </c>
+      <c r="N30">
+        <v>0.82</v>
+      </c>
+      <c r="O30">
+        <v>0.77</v>
+      </c>
+      <c r="P30">
+        <v>0.81</v>
+      </c>
+      <c r="Q30">
+        <v>0.96</v>
+      </c>
+      <c r="W30">
+        <v>9</v>
+      </c>
+      <c r="X30">
+        <v>0.81</v>
+      </c>
+      <c r="Y30">
+        <v>0.79</v>
+      </c>
+      <c r="Z30">
+        <v>0.75</v>
+      </c>
+      <c r="AA30">
+        <v>0.78</v>
+      </c>
+      <c r="AB30">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>0.72</v>
+      </c>
+      <c r="C31">
+        <v>0.73</v>
+      </c>
+      <c r="D31">
+        <v>0.68</v>
+      </c>
+      <c r="E31">
+        <v>0.71</v>
+      </c>
+      <c r="F31">
+        <v>0.76</v>
+      </c>
+      <c r="L31">
+        <v>10</v>
+      </c>
+      <c r="M31">
+        <v>0.81</v>
+      </c>
+      <c r="N31">
+        <v>0.79</v>
+      </c>
+      <c r="O31">
+        <v>0.8</v>
+      </c>
+      <c r="P31">
+        <v>0.8</v>
+      </c>
+      <c r="Q31">
+        <v>0.81</v>
+      </c>
+      <c r="W31">
+        <v>10</v>
+      </c>
+      <c r="X31">
+        <v>0.8</v>
+      </c>
+      <c r="Y31">
+        <v>0.74</v>
+      </c>
+      <c r="Z31">
+        <v>0.77</v>
+      </c>
+      <c r="AA31">
+        <v>0.78</v>
+      </c>
+      <c r="AB31">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>11</v>
+      </c>
+      <c r="B32">
+        <v>0.72</v>
+      </c>
+      <c r="C32">
+        <v>0.76</v>
+      </c>
+      <c r="D32">
+        <v>0.76</v>
+      </c>
+      <c r="E32">
+        <v>0.67</v>
+      </c>
+      <c r="F32">
+        <v>0.81</v>
+      </c>
+      <c r="L32">
+        <v>11</v>
+      </c>
+      <c r="M32">
+        <v>0.8</v>
+      </c>
+      <c r="N32">
+        <v>0.81</v>
+      </c>
+      <c r="O32">
+        <v>0.79</v>
+      </c>
+      <c r="P32">
+        <v>0.81</v>
+      </c>
+      <c r="Q32">
+        <v>0.8</v>
+      </c>
+      <c r="W32">
+        <v>11</v>
+      </c>
+      <c r="X32">
+        <v>0.76</v>
+      </c>
+      <c r="Y32">
+        <v>0.79</v>
+      </c>
+      <c r="Z32">
+        <v>0.79</v>
+      </c>
+      <c r="AA32">
+        <v>0.75</v>
+      </c>
+      <c r="AB32">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>12</v>
+      </c>
+      <c r="B33">
+        <v>0.73</v>
+      </c>
+      <c r="C33">
+        <v>0.85</v>
+      </c>
+      <c r="D33">
+        <v>0.71</v>
+      </c>
+      <c r="E33">
+        <v>0.83</v>
+      </c>
+      <c r="F33">
+        <v>0.68</v>
+      </c>
+      <c r="L33">
+        <v>12</v>
+      </c>
+      <c r="M33">
+        <v>0.79</v>
+      </c>
+      <c r="N33">
+        <v>0.81</v>
+      </c>
+      <c r="O33">
+        <v>0.81</v>
+      </c>
+      <c r="P33">
+        <v>0.83</v>
+      </c>
+      <c r="Q33">
+        <v>0.8</v>
+      </c>
+      <c r="W33">
+        <v>12</v>
+      </c>
+      <c r="X33">
+        <v>0.75</v>
+      </c>
+      <c r="Y33">
+        <v>0.77</v>
+      </c>
+      <c r="Z33">
+        <v>0.76</v>
+      </c>
+      <c r="AA33">
+        <v>0.89</v>
+      </c>
+      <c r="AB33">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34">
+        <f>MAX(B22:F33)</f>
+        <v>0.94</v>
+      </c>
+      <c r="C34">
+        <f>MIN(B22:F33)</f>
+        <v>0.59</v>
+      </c>
+      <c r="L34" t="s">
+        <v>21</v>
+      </c>
+      <c r="M34">
+        <f>MAX(M22:Q33)</f>
+        <v>0.96</v>
+      </c>
+      <c r="N34">
+        <f>MIN(M22:Q33)</f>
+        <v>0.77</v>
+      </c>
+      <c r="W34" t="s">
+        <v>21</v>
+      </c>
+      <c r="X34">
+        <f>MAX(X22:AB33)</f>
+        <v>0.96</v>
+      </c>
+      <c r="Y34">
+        <f>MIN(X22:AB33)</f>
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="X35" s="1"/>
+      <c r="Y35" s="1"/>
+      <c r="Z35" s="1"/>
+      <c r="AA35" s="1"/>
+      <c r="AB35" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="L2:S2"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="L20:S20"/>
+    <mergeCell ref="W20:AD20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>